<commit_message>
AW-Datapipeline_Tasks_Phase1.sql   Book1.xlsx, AW-Datapipeline_Tasks_image.jpg 'CAPSTONE_PROJECT 3.pdf', Vies.sql
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="210">
   <si>
     <t>FieldName</t>
   </si>
@@ -645,6 +645,9 @@
   </si>
   <si>
     <t>Date of first purchase</t>
+  </si>
+  <si>
+    <t>ADV_CustomerKey</t>
   </si>
 </sst>
 </file>
@@ -1684,7 +1687,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1730,7 +1733,7 @@
         <v>156</v>
       </c>
       <c r="C2" t="s">
-        <v>127</v>
+        <v>209</v>
       </c>
       <c r="D2" t="s">
         <v>45</v>

</xml_diff>